<commit_message>
Semana 5 | dia 3 | Inclusion de los KPIs
</commit_message>
<xml_diff>
--- a/1_business_understanding_module/kpis diseño.xlsx
+++ b/1_business_understanding_module/kpis diseño.xlsx
@@ -147,7 +147,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="$#,##0_);($#,##0)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +161,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -171,6 +177,13 @@
     </fill>
   </fills>
   <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -193,59 +206,70 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -562,289 +586,289 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="15" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="15" width="12.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="10" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="10" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="10" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="16" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="21" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="21" width="12.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="15" width="10.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="13" width="10.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="15" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="13" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="15" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="22" width="17.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="16" t="s">
         <v>16</v>
       </c>
       <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="16" t="s">
         <v>17</v>
       </c>
       <c r="J1" s="2"/>
-      <c r="K1" s="13"/>
+      <c r="K1" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="19" t="s">
         <v>26</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="9">
         <v>120</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="9">
         <v>20</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="9">
         <f>+E3*F3</f>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="9">
         <v>120</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="9">
         <f>+H3*E3</f>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="9">
         <v>2</v>
       </c>
-      <c r="K3" s="14">
+      <c r="K3" s="20">
         <f>+E3/'diseño extraccion seguidores'!E3</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="9">
         <v>20</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="9">
         <v>20</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="9">
         <f>+E4*F4</f>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="9">
         <v>450</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="9">
         <f>+H4*E4</f>
       </c>
       <c r="J4" s="2"/>
-      <c r="K4" s="13"/>
+      <c r="K4" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="9">
         <f>+E4+23</f>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="9">
         <v>40</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="9">
         <f>+E5*F5</f>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="9">
         <v>450</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="9">
         <f>+H5*E5</f>
       </c>
       <c r="J5" s="2"/>
-      <c r="K5" s="13"/>
+      <c r="K5" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="9">
         <f>+E5+23</f>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="9">
         <v>40</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="9">
         <f>+E6*F6</f>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="9">
         <v>100</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="9">
         <f>+H6*E6</f>
       </c>
       <c r="J6" s="2"/>
-      <c r="K6" s="13"/>
+      <c r="K6" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="9">
         <v>12</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="9">
         <v>40</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="9">
         <f>+E7*F7</f>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="9">
         <v>450</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="9">
         <f>+H7*E7</f>
       </c>
       <c r="J7" s="2"/>
-      <c r="K7" s="13"/>
+      <c r="K7" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="9">
         <v>51</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="9">
         <v>20</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="9">
         <f>+E8*F8</f>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="9">
         <v>450</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="9">
         <f>+H8*E8</f>
       </c>
       <c r="J8" s="2"/>
-      <c r="K8" s="13"/>
+      <c r="K8" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="13"/>
+      <c r="K9" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="12" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="12"/>
+      <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="13"/>
+      <c r="K10" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="2" t="s">
         <v>40</v>
       </c>
       <c r="F11" s="2"/>
@@ -852,18 +876,18 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="13"/>
+      <c r="K11" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1" t="s">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="9">
         <v>2</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="9">
         <v>1000</v>
       </c>
       <c r="F12" s="2"/>
@@ -871,18 +895,18 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="13"/>
+      <c r="K12" s="17"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1" t="s">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="9">
         <v>50</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="9">
         <v>70</v>
       </c>
       <c r="F13" s="2"/>
@@ -890,7 +914,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="13"/>
+      <c r="K13" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -908,14 +932,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="23.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="23.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="15" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -926,106 +950,106 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="7">
         <v>250</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="7">
         <v>500</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="7">
         <f>+C3+D3</f>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="7">
+      <c r="F3" s="3"/>
+      <c r="G3" s="8">
         <v>60</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="9">
         <f>60*10</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="3"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="10"/>
       <c r="H4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="3"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="10"/>
       <c r="H5" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="3"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="10"/>
       <c r="H6" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="3"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="10"/>
       <c r="H7" s="2"/>
     </row>
   </sheetData>

</xml_diff>